<commit_message>
fix(horizon): update proper dataset from excel (741 calls) and add guide
</commit_message>
<xml_diff>
--- a/horizon-reports/horizon_rapor_latest.xlsx
+++ b/horizon-reports/horizon_rapor_latest.xlsx
@@ -12,7 +12,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tüm Açık Çağrılar" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Yeni Açılan Çağrılar'!$A$1:$E$40</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Tüm Misyon Çağrıları'!$A$1:$E$70</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Tüm Açık Çağrılar'!$A$1:$E$742</definedName>
   </definedNames>
@@ -441,7 +440,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,867 +483,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>Testing and optimising models of co-creation of advanced research infrastructure technologies</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-TECH-01-01</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E2" s="4" t="n">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Strengthening the potential of the EOSC for knowledge valorisation and industry-academia collaboration (EOSC Partnership)</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-01-EOSC-02</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Preparatory phase of new ESFRI research infrastructure projects</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-DEV-01-01</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E4" s="4" t="n">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Expanding and deepening the EOSC Federation (EOSC Partnership)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-01-EOSC-01</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E5" s="4" t="n">
-        <v>40000000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Access to research infrastructure services to enable R&amp;I addressing EU priorities and emerging challenges</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-SERV-01-02</t>
-        </is>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Access to research infrastructures, their resources and services: large-scale pilots for more integrated scheme across (sub)domains</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-SERV-01-01</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>35000000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Connecting research infrastructures and a wider user community across the European Research Area through access to advanced research infrastructure services</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-SERV-01-03</t>
-        </is>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="inlineStr">
-        <is>
-          <t>Pioneering Destination Earth for a Sustainable Future: Large-Scale Pilots and Demonstrators</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-TECH-01-02</t>
-        </is>
-      </c>
-      <c r="C9" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="inlineStr">
-        <is>
-          <t>Consolidation of the research infrastructure landscape – individual support for evolution, long-term sustainability and emerging needs of pan-European research infrastructures</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>HORIZON-INFRA-2027-DEV-01-03</t>
-        </is>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>46455</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>46553</v>
-      </c>
-      <c r="E10" s="4" t="n">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
-        <is>
-          <t>Pillar I: Facilitating development of institutional open access policies through the retention of intellectual property rights</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>HORIZON-WIDERA-2027-05-ERA-01</t>
-        </is>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>46364</v>
-      </c>
-      <c r="D11" s="3" t="n">
-        <v>46457</v>
-      </c>
-      <c r="E11" s="4" t="n">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Pillar IV: Upgrading the EU’s independent knowledge on China's Science, Technology and Innovation system</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>HORIZON-WIDERA-2027-05-ERA-05</t>
-        </is>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>46364</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>46457</v>
-      </c>
-      <c r="E12" s="4" t="n">
-        <v>3000000</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>Pillar III: Science comes to town 2029</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>HORIZON-WIDERA-2027-05-ERA-03</t>
-        </is>
-      </c>
-      <c r="C13" s="3" t="n">
-        <v>46364</v>
-      </c>
-      <c r="D13" s="3" t="n">
-        <v>46457</v>
-      </c>
-      <c r="E13" s="4" t="n">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Pillar III: Promoting public engagement in R&amp;I and scientific literacy</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>HORIZON-WIDERA-2027-05-ERA-04</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>46364</v>
-      </c>
-      <c r="D14" s="3" t="n">
-        <v>46457</v>
-      </c>
-      <c r="E14" s="4" t="n">
-        <v>1000000</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>Pillar II: Talent ecosystems for attractive early research careers</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>HORIZON-WIDERA-2027-05-ERA-02</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="n">
-        <v>46364</v>
-      </c>
-      <c r="D15" s="3" t="n">
-        <v>46457</v>
-      </c>
-      <c r="E15" s="4" t="n">
-        <v>2000000</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Demonstrating solutions to protect and preserve cultural heritage from the impacts of climate change</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-01-CLIMA-05</t>
-        </is>
-      </c>
-      <c r="C16" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D16" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E16" s="4" t="n">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>Standardising and supporting climate services for  climate adaptation</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-01-CLIMA-03</t>
-        </is>
-      </c>
-      <c r="C17" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D17" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E17" s="4" t="n">
-        <v>9000000</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Improving climate resilience of navigable inland waterways, their surroundings and related water infrastructure</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-01-CLIMA-06</t>
-        </is>
-      </c>
-      <c r="C18" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D18" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E18" s="4" t="n">
-        <v>6000000</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Addressing aquatic pollution and biodiversity loss through nature positive solutions from source to sea</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-03-OCEAN-02</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E19" s="4" t="n">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>Large-scale demonstration for mapping the distribution and condition of marine habitats to implement the Nature Restoration Regulation</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-03-OCEAN-01</t>
-        </is>
-      </c>
-      <c r="C20" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D20" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E20" s="4" t="n">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Supporting financing of local adaptation actions with combination of public funding and private financing</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-01-CLIMA-07</t>
-        </is>
-      </c>
-      <c r="C21" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D21" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E21" s="4" t="n">
-        <v>20000000</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Regional  (sea-basins) components of the EU Digital Twin Ocean</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-03-OCEAN-05</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E22" s="4" t="n">
-        <v>4000000</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>Towards a European network of ocean technology testing sites</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-03-OCEAN-04</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D23" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E23" s="4" t="n">
-        <v>2500000</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>National Adaptation Hubs - Bringing together the national level with the engaged regional and local levels (multi-level governance)</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-01-CLIMA-01</t>
-        </is>
-      </c>
-      <c r="C24" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D24" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E24" s="4" t="n">
-        <v>10000000</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>Facilitating implementation of actionable solutions for climate adaptation of regions and local authorities</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-01-CLIMA-02</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E25" s="4" t="n">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>Bridging the gap between disaster risk management and climate adaptation</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-01-CLIMA-04</t>
-        </is>
-      </c>
-      <c r="C26" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D26" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E26" s="4" t="n">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>By fishers, for fishers: co-management of marine and freshwaters ecosystems and resources</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2026-03-OCEAN-03</t>
-        </is>
-      </c>
-      <c r="C27" s="3" t="n">
-        <v>46057</v>
-      </c>
-      <c r="D27" s="3" t="n">
-        <v>46288</v>
-      </c>
-      <c r="E27" s="4" t="n">
-        <v>7000000</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>RAPTOR 2026 Open Call</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>HORIZON-EIT-2025-KIC-IBA-UM</t>
-        </is>
-      </c>
-      <c r="C28" s="3" t="n">
-        <v>46038</v>
-      </c>
-      <c r="D28" s="3" t="n">
-        <v>46093.70833333334</v>
-      </c>
-      <c r="E28" s="4" t="n">
-        <v>900000</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>Call 1 – “Collection &amp; Valorisation”</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>HORIZON-MISS-2022-OCEAN-01-04</t>
-        </is>
-      </c>
-      <c r="C29" s="3" t="n">
-        <v>46037</v>
-      </c>
-      <c r="D29" s="3" t="n">
-        <v>46097.70833333334</v>
-      </c>
-      <c r="E29" s="4" t="n">
-        <v>210000</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>Boosting innovation through better integration of fragmented health R&amp;I efforts</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-IHI-2026-12-SINGLE-STAGE-02</t>
-        </is>
-      </c>
-      <c r="C30" s="3" t="n">
-        <v>46037</v>
-      </c>
-      <c r="D30" s="3" t="n">
-        <v>46133</v>
-      </c>
-      <c r="E30" s="4" t="n">
-        <v>15000000</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>Boosting innovation for a better understanding of the determinants of health</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-IHI-2026-12-SINGLE-STAGE-01</t>
-        </is>
-      </c>
-      <c r="C31" s="3" t="n">
-        <v>46037</v>
-      </c>
-      <c r="D31" s="3" t="n">
-        <v>46133</v>
-      </c>
-      <c r="E31" s="4" t="n">
-        <v>8000000</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>Boosting innovation for people-centred integrated healthcare solutions</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-IHI-2026-12-SINGLE-STAGE-03</t>
-        </is>
-      </c>
-      <c r="C32" s="3" t="n">
-        <v>46037</v>
-      </c>
-      <c r="D32" s="3" t="n">
-        <v>46133</v>
-      </c>
-      <c r="E32" s="4" t="n">
-        <v>8000000</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>Boosting innovation through exploitation of digitalisation and data exchange in healthcare</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-IHI-2026-12-SINGLE-STAGE-04</t>
-        </is>
-      </c>
-      <c r="C33" s="3" t="n">
-        <v>46037</v>
-      </c>
-      <c r="D33" s="3" t="n">
-        <v>46133</v>
-      </c>
-      <c r="E33" s="4" t="n">
-        <v>8000000</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="inlineStr">
-        <is>
-          <t>Boosting innovation for better assessment of the added value of innovative integrated healthcare solutions</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-IHI-2026-12-SINGLE-STAGE-05</t>
-        </is>
-      </c>
-      <c r="C34" s="3" t="n">
-        <v>46037</v>
-      </c>
-      <c r="D34" s="3" t="n">
-        <v>46133</v>
-      </c>
-      <c r="E34" s="4" t="n">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="inlineStr">
-        <is>
-          <t>Global collaboration action for prevention and treatment of Lower Respiratory Tract Infections (LRTIs) in sub-Saharan Africa</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-GH-EDCTP3-2026-01-LRTI-02-two-stage</t>
-        </is>
-      </c>
-      <c r="C35" s="3" t="n">
-        <v>46036</v>
-      </c>
-      <c r="D35" s="3" t="n">
-        <v>46282</v>
-      </c>
-      <c r="E35" s="4" t="n">
-        <v>8475000</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="inlineStr">
-        <is>
-          <t>Global collaboration action towards better prevention, treatment and clinical management of HIV co-infections or co-morbidities in sub-Saharan Africa</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-GH-EDCTP3-2026-01-HIV-03-two-stage</t>
-        </is>
-      </c>
-      <c r="C36" s="3" t="n">
-        <v>46036</v>
-      </c>
-      <c r="D36" s="3" t="n">
-        <v>46282</v>
-      </c>
-      <c r="E36" s="4" t="n">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="inlineStr">
-        <is>
-          <t>Global collaboration action on climate and health in sub-Saharan Africa</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-GH-EDCTP3-2026-02-CH-01-two-stage</t>
-        </is>
-      </c>
-      <c r="C37" s="3" t="n">
-        <v>46036</v>
-      </c>
-      <c r="D37" s="3" t="n">
-        <v>46282</v>
-      </c>
-      <c r="E37" s="4" t="n">
-        <v>5000000</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="inlineStr">
-        <is>
-          <t>Training and innovation networks for sustained capacity development related to ethics, regulatory, pharmacovigilance, and related digital regulatory platforms</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-GH-EDCTP3-2026-03-SERP-01</t>
-        </is>
-      </c>
-      <c r="C38" s="3" t="n">
-        <v>46036</v>
-      </c>
-      <c r="D38" s="3" t="n">
-        <v>46267</v>
-      </c>
-      <c r="E38" s="4" t="n">
-        <v>1500000</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="2" t="inlineStr">
-        <is>
-          <t>Enhancing integrated research and healthcare in sub-Saharan Africa through digital innovation and Artificial Intelligence</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-GH-EDCTP3-2026-03-DIGIT-02</t>
-        </is>
-      </c>
-      <c r="C39" s="3" t="n">
-        <v>46036</v>
-      </c>
-      <c r="D39" s="3" t="n">
-        <v>46267</v>
-      </c>
-      <c r="E39" s="4" t="n">
-        <v>2250000</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="inlineStr">
-        <is>
-          <t>Global collaboration action for the development of TB drugs for therapy and chemoprophylaxis in adults and children in sub-Saharan Africa</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>HORIZON-JU-GH-EDCTP3-2026-01-TB-01-two-stage</t>
-        </is>
-      </c>
-      <c r="C40" s="3" t="n">
-        <v>46036</v>
-      </c>
-      <c r="D40" s="3" t="n">
-        <v>46282</v>
-      </c>
-      <c r="E40" s="4" t="n">
-        <v>10000000</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Bu hafta yeni açılan çağrı bulunmamaktadır.</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E40"/>
-  <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A2" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A3" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A4" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A5" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A6" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A7" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A8" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A9" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A10" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A11" r:id="rId10"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A12" r:id="rId11"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A13" r:id="rId12"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A14" r:id="rId13"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A15" r:id="rId14"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A16" r:id="rId15"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A17" r:id="rId16"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A18" r:id="rId17"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A19" r:id="rId18"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A20" r:id="rId19"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A21" r:id="rId20"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A22" r:id="rId21"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A23" r:id="rId22"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A24" r:id="rId23"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A25" r:id="rId24"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A26" r:id="rId25"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A27" r:id="rId26"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A28" r:id="rId27"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A29" r:id="rId28"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A30" r:id="rId29"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A31" r:id="rId30"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A32" r:id="rId31"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A33" r:id="rId32"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A34" r:id="rId33"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A35" r:id="rId34"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A36" r:id="rId35"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A37" r:id="rId36"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A38" r:id="rId37"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A39" r:id="rId38"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="A40" r:id="rId39"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -7165,12 +6310,12 @@
     <row r="202">
       <c r="A202" s="2" t="inlineStr">
         <is>
-          <t>Production technologies for solar photovoltaics beyond the state-of-the-art (EUPI-PV Partnership)</t>
+          <t>Large scale operational validation and upscaling of state-of-the-art (Generative) AI tools and models powering a next generation digital energy system</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2027-02-D3-15</t>
+          <t>HORIZON-CL5-2027-02-D3-24</t>
         </is>
       </c>
       <c r="C202" s="3" t="n">
@@ -7180,18 +6325,18 @@
         <v>46477</v>
       </c>
       <c r="E202" s="4" t="n">
-        <v>12000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="2" t="inlineStr">
         <is>
-          <t>Support to the implementation of an EU policy framework for CO2 transport and storage infrastructure</t>
+          <t>Production technologies for solar photovoltaics beyond the state-of-the-art (EUPI-PV Partnership)</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2027-02-D3-31</t>
+          <t>HORIZON-CL5-2027-02-D3-15</t>
         </is>
       </c>
       <c r="C203" s="3" t="n">
@@ -7201,18 +6346,18 @@
         <v>46477</v>
       </c>
       <c r="E203" s="4" t="n">
-        <v>5000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="2" t="inlineStr">
         <is>
-          <t>Large scale operational validation and upscaling of state-of-the-art (Generative) AI tools and models powering a next generation digital energy system</t>
+          <t>Advancements in Direct Air Capture</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2027-02-D3-24</t>
+          <t>HORIZON-CL5-2027-02-D3-30</t>
         </is>
       </c>
       <c r="C204" s="3" t="n">
@@ -7222,18 +6367,18 @@
         <v>46477</v>
       </c>
       <c r="E204" s="4" t="n">
-        <v>10000000</v>
+        <v>8000000</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="2" t="inlineStr">
         <is>
-          <t>Advancements in Direct Air Capture</t>
+          <t>Sustainable and Competitive Cell Production Techniques for Lithium-ion And Sodium-ion Batteries (BATT4EU Partnership)</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2027-02-D3-30</t>
+          <t>HORIZON-CL5-2027-02-D2-06</t>
         </is>
       </c>
       <c r="C205" s="3" t="n">
@@ -7243,7 +6388,7 @@
         <v>46477</v>
       </c>
       <c r="E205" s="4" t="n">
-        <v>8000000</v>
+        <v>18900000</v>
       </c>
     </row>
     <row r="206">
@@ -7333,12 +6478,12 @@
     <row r="210">
       <c r="A210" s="2" t="inlineStr">
         <is>
-          <t>Demand-side 3C pilot demonstrators on converged Telco Edge Cloud Infrastructure (IA)</t>
+          <t>Apply AI: AI-Driven Robotics for Industry: Enabling System Integration and Adoption (IA) (Partnership in AI, Data and Robotics)</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-DATA-08</t>
+          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-05</t>
         </is>
       </c>
       <c r="C210" s="3" t="n">
@@ -7348,18 +6493,18 @@
         <v>46464</v>
       </c>
       <c r="E210" s="4" t="n">
-        <v>19000000</v>
+        <v>18000000</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="inlineStr">
         <is>
-          <t>Facilitate the engagement of European stakeholders in international digital standardisation (CSA)</t>
+          <t>Demand-side 3C pilot demonstrators on converged Telco Edge Cloud Infrastructure (IA)</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-HUMAN-07</t>
+          <t>HORIZON-CL4-2027-04-DATA-08</t>
         </is>
       </c>
       <c r="C211" s="3" t="n">
@@ -7369,18 +6514,18 @@
         <v>46464</v>
       </c>
       <c r="E211" s="4" t="n">
-        <v>7000000</v>
+        <v>19000000</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="2" t="inlineStr">
         <is>
-          <t>Energy efficiency and sustainability of AI data processing in Data Centres (IA)</t>
+          <t>New approaches for decentralized, federated and sustainable AI data processing (RIA)</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-DATA-09</t>
+          <t>HORIZON-CL4-2027-04-DATA-03</t>
         </is>
       </c>
       <c r="C212" s="3" t="n">
@@ -7390,18 +6535,18 @@
         <v>46464</v>
       </c>
       <c r="E212" s="4" t="n">
-        <v>10000000</v>
+        <v>17500000</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="inlineStr">
         <is>
-          <t>Advanced and Innovative hardware components for Virtual Worlds (RIA) (Virtual Worlds Partnership)</t>
+          <t>Facilitate the engagement of European stakeholders in international digital standardisation (CSA)</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-HUMAN-01</t>
+          <t>HORIZON-CL4-2027-04-HUMAN-07</t>
         </is>
       </c>
       <c r="C213" s="3" t="n">
@@ -7411,18 +6556,18 @@
         <v>46464</v>
       </c>
       <c r="E213" s="4" t="n">
-        <v>4800000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="inlineStr">
         <is>
-          <t>Create a thriving and competitive Virtual Worlds and Web 4.0 ecosystem (CSA) (Virtual Worlds Partnership)</t>
+          <t>Energy efficiency and sustainability of AI data processing in Data Centres (IA)</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-HUMAN-02</t>
+          <t>HORIZON-CL4-2027-04-DATA-09</t>
         </is>
       </c>
       <c r="C214" s="3" t="n">
@@ -7432,18 +6577,18 @@
         <v>46464</v>
       </c>
       <c r="E214" s="4" t="n">
-        <v>3000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="2" t="inlineStr">
         <is>
-          <t>EU Frontier AI Initiative:  Developing frontier AI solutions that are safe and computationally efficient within Apply AI (RIA)</t>
+          <t>International cooperation in AI (IA)</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-11</t>
+          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-06</t>
         </is>
       </c>
       <c r="C215" s="3" t="n">
@@ -7453,18 +6598,18 @@
         <v>46464</v>
       </c>
       <c r="E215" s="4" t="n">
-        <v>44000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="inlineStr">
         <is>
-          <t>Horizon scanning and foresight in future enabling digital technologies (CSA)</t>
+          <t>Advanced and Innovative hardware components for Virtual Worlds (RIA) (Virtual Worlds Partnership)</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-10</t>
+          <t>HORIZON-CL4-2027-04-HUMAN-01</t>
         </is>
       </c>
       <c r="C216" s="3" t="n">
@@ -7474,18 +6619,18 @@
         <v>46464</v>
       </c>
       <c r="E216" s="4" t="n">
-        <v>4000000</v>
+        <v>4800000</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="inlineStr">
         <is>
-          <t>Apply AI: AI-Driven Robotics for Industry: Enabling System Integration and Adoption (IA) (Partnership in AI, Data and Robotics)</t>
+          <t>Create a thriving and competitive Virtual Worlds and Web 4.0 ecosystem (CSA) (Virtual Worlds Partnership)</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-05</t>
+          <t>HORIZON-CL4-2027-04-HUMAN-02</t>
         </is>
       </c>
       <c r="C217" s="3" t="n">
@@ -7495,18 +6640,18 @@
         <v>46464</v>
       </c>
       <c r="E217" s="4" t="n">
-        <v>18000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="inlineStr">
         <is>
-          <t>New approaches for decentralized, federated and sustainable AI data processing (RIA)</t>
+          <t>EU Frontier AI Initiative:  Developing frontier AI solutions that are safe and computationally efficient within Apply AI (RIA)</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-DATA-03</t>
+          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-11</t>
         </is>
       </c>
       <c r="C218" s="3" t="n">
@@ -7516,18 +6661,18 @@
         <v>46464</v>
       </c>
       <c r="E218" s="4" t="n">
-        <v>17500000</v>
+        <v>44000000</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="2" t="inlineStr">
         <is>
-          <t>International cooperation in AI (IA)</t>
+          <t>Horizon scanning and foresight in future enabling digital technologies (CSA)</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-06</t>
+          <t>HORIZON-CL4-2027-04-DIGITAL-EMERGING-10</t>
         </is>
       </c>
       <c r="C219" s="3" t="n">
@@ -7537,7 +6682,7 @@
         <v>46464</v>
       </c>
       <c r="E219" s="4" t="n">
-        <v>1500000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="220">
@@ -7564,12 +6709,12 @@
     <row r="221">
       <c r="A221" s="2" t="inlineStr">
         <is>
-          <t>Fast Track to Innovation for breakthroughs in the Chemical Industry Action Plan  (Research and Innovation Action)</t>
+          <t>Unlocking the potential of academic intellectual assets for industry, SMEs and startups (CSA)</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-62</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-42</t>
         </is>
       </c>
       <c r="C221" s="3" t="n">
@@ -7578,6 +6723,9 @@
       <c r="D221" s="3" t="n">
         <v>46420</v>
       </c>
+      <c r="E221" s="4" t="n">
+        <v>1000000</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="inlineStr">
@@ -7603,12 +6751,12 @@
     <row r="223">
       <c r="A223" s="2" t="inlineStr">
         <is>
-          <t>Unlocking the potential of academic intellectual assets for industry, SMEs and startups (CSA)</t>
+          <t>Fast Track to Research and Innovation for breakthroughs in industrial technologies (Research and Innovation Action)</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-42</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-61</t>
         </is>
       </c>
       <c r="C223" s="3" t="n">
@@ -7617,19 +6765,16 @@
       <c r="D223" s="3" t="n">
         <v>46420</v>
       </c>
-      <c r="E223" s="4" t="n">
-        <v>1000000</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="inlineStr">
         <is>
-          <t>Fast Track to Research and Innovation for breakthroughs in industrial technologies (Research and Innovation Action)</t>
+          <t>Fast Track to Innovation for breakthroughs in the Chemical Industry Action Plan  (Research and Innovation Action)</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-61</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-62</t>
         </is>
       </c>
       <c r="C224" s="3" t="n">
@@ -7642,33 +6787,33 @@
     <row r="225">
       <c r="A225" s="2" t="inlineStr">
         <is>
-          <t>Expert network on Critical raw materials (CSA)</t>
+          <t>Efficient energy input from renewable sources and energy management in the process industries (IA) (Processes4Planet and Innovative Advanced Materials for the EU partnerships)</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-17</t>
+          <t>HORIZON-CL4-2027-02-MAT-PROD-32-two-stage</t>
         </is>
       </c>
       <c r="C225" s="3" t="n">
         <v>46287</v>
       </c>
       <c r="D225" s="3" t="n">
-        <v>46420</v>
+        <v>46632</v>
       </c>
       <c r="E225" s="4" t="n">
-        <v>3000000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="2" t="inlineStr">
         <is>
-          <t>Circular innovative advanced materials: facilitating the transition from design to markets (RIA) (Innovative Advanced Materials for the EU and Made in Europe partnerships)</t>
+          <t>Automated Scientific Discovery (RAISE pilot) (RIA)</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-06</t>
+          <t>HORIZON-RAISE-2027-01-01</t>
         </is>
       </c>
       <c r="C226" s="3" t="n">
@@ -7678,18 +6823,18 @@
         <v>46420</v>
       </c>
       <c r="E226" s="4" t="n">
-        <v>5000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="inlineStr">
         <is>
-          <t>Innovative advanced materials and new production processes – reducing dependencies on Critical and Strategic Raw Materials (IA) (Innovative Advanced Materials for the EU and Processes4Planet partnerships)</t>
+          <t>Pilot access schemes to Technology Infrastructures for European startups, scaleups and innovative SMEs (CSA)</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-22</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-47</t>
         </is>
       </c>
       <c r="C227" s="3" t="n">
@@ -7699,7 +6844,7 @@
         <v>46420</v>
       </c>
       <c r="E227" s="4" t="n">
-        <v>6000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="228">
@@ -7747,12 +6892,12 @@
     <row r="230">
       <c r="A230" s="2" t="inlineStr">
         <is>
-          <t>Automated Scientific Discovery (RAISE pilot) (RIA)</t>
+          <t>‘Proof of market’ to improve valorisation and commercialisation of Horizon generated R&amp;I results (IA)</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>HORIZON-RAISE-2027-01-01</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-49</t>
         </is>
       </c>
       <c r="C230" s="3" t="n">
@@ -7762,18 +6907,18 @@
         <v>46420</v>
       </c>
       <c r="E230" s="4" t="n">
-        <v>10000000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="2" t="inlineStr">
         <is>
-          <t>Automated Scientific Discovery – Food (RAISE pilot)</t>
+          <t>Technologies for innovative processing of raw materials (IA)</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>HORIZON-RAISE-2027-01-02</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-16</t>
         </is>
       </c>
       <c r="C231" s="3" t="n">
@@ -7783,39 +6928,39 @@
         <v>46420</v>
       </c>
       <c r="E231" s="4" t="n">
-        <v>3000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="2" t="inlineStr">
         <is>
-          <t>Efficient energy input from renewable sources and energy management in the process industries (IA) (Processes4Planet and Innovative Advanced Materials for the EU partnerships)</t>
+          <t>Automated Scientific Discovery – Food (RAISE pilot)</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-02-MAT-PROD-32-two-stage</t>
+          <t>HORIZON-RAISE-2027-01-02</t>
         </is>
       </c>
       <c r="C232" s="3" t="n">
         <v>46287</v>
       </c>
       <c r="D232" s="3" t="n">
-        <v>46632</v>
+        <v>46420</v>
       </c>
       <c r="E232" s="4" t="n">
-        <v>7000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="inlineStr">
         <is>
-          <t>Technologies for innovative processing of raw materials (IA)</t>
+          <t>Expert network on Critical raw materials (CSA)</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-16</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-17</t>
         </is>
       </c>
       <c r="C233" s="3" t="n">
@@ -7825,18 +6970,18 @@
         <v>46420</v>
       </c>
       <c r="E233" s="4" t="n">
-        <v>10000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="inlineStr">
         <is>
-          <t>‘Proof of market’ to improve valorisation and commercialisation of Horizon generated R&amp;I results (IA)</t>
+          <t>Innovative advanced materials and new production processes – reducing dependencies on Critical and Strategic Raw Materials (IA) (Innovative Advanced Materials for the EU and Processes4Planet partnerships)</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-49</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-22</t>
         </is>
       </c>
       <c r="C234" s="3" t="n">
@@ -7846,18 +6991,18 @@
         <v>46420</v>
       </c>
       <c r="E234" s="4" t="n">
-        <v>200000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="2" t="inlineStr">
         <is>
-          <t>Pilot access schemes to Technology Infrastructures for European startups, scaleups and innovative SMEs (CSA)</t>
+          <t>Circular innovative advanced materials: facilitating the transition from design to markets (RIA) (Innovative Advanced Materials for the EU and Made in Europe partnerships)</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2027-01-MAT-PROD-47</t>
+          <t>HORIZON-CL4-2027-01-MAT-PROD-06</t>
         </is>
       </c>
       <c r="C235" s="3" t="n">
@@ -7867,7 +7012,7 @@
         <v>46420</v>
       </c>
       <c r="E235" s="4" t="n">
-        <v>1500000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="236">
@@ -8041,12 +7186,12 @@
     <row r="244">
       <c r="A244" s="2" t="inlineStr">
         <is>
-          <t>Increasing competitiveness and resilience of multimodal freight transport and logistics for competitive supply chains</t>
+          <t>Flagship-pilot: large-scale demonstrations of CCAM (CCAM Partnership)</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-10-D6-06</t>
+          <t>HORIZON-CL5-2026-10-D6-01</t>
         </is>
       </c>
       <c r="C244" s="3" t="n">
@@ -8056,7 +7201,7 @@
         <v>46303</v>
       </c>
       <c r="E244" s="4" t="n">
-        <v>6500000</v>
+        <v>100000000</v>
       </c>
     </row>
     <row r="245">
@@ -8125,12 +7270,12 @@
     <row r="248">
       <c r="A248" s="2" t="inlineStr">
         <is>
-          <t>Supporting sustainable and smart urban mobility in Europe (CIVITAS)</t>
+          <t>Generative AI for smarter CCAM: enhancing perception, decision-making, and validation (CCAM Partnership)</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-10-D6-07</t>
+          <t>HORIZON-CL5-2026-10-D6-03</t>
         </is>
       </c>
       <c r="C248" s="3" t="n">
@@ -8140,18 +7285,18 @@
         <v>46303</v>
       </c>
       <c r="E248" s="4" t="n">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" s="2" t="inlineStr">
         <is>
-          <t>Flagship-pilot: large-scale demonstrations of CCAM (CCAM Partnership)</t>
+          <t>Increasing competitiveness and resilience of multimodal freight transport and logistics for competitive supply chains</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-10-D6-01</t>
+          <t>HORIZON-CL5-2026-10-D6-06</t>
         </is>
       </c>
       <c r="C249" s="3" t="n">
@@ -8161,18 +7306,18 @@
         <v>46303</v>
       </c>
       <c r="E249" s="4" t="n">
-        <v>100000000</v>
+        <v>6500000</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" s="2" t="inlineStr">
         <is>
-          <t>Generative AI for smarter CCAM: enhancing perception, decision-making, and validation (CCAM Partnership)</t>
+          <t>Supporting sustainable and smart urban mobility in Europe (CIVITAS)</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-10-D6-03</t>
+          <t>HORIZON-CL5-2026-10-D6-07</t>
         </is>
       </c>
       <c r="C250" s="3" t="n">
@@ -8182,7 +7327,7 @@
         <v>46303</v>
       </c>
       <c r="E250" s="4" t="n">
-        <v>6500000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="251">
@@ -9253,12 +8398,12 @@
     <row r="302">
       <c r="A302" s="2" t="inlineStr">
         <is>
-          <t>Producing battery-grade materials for electrodes through sustainable processing and refining of raw materials or developing bio-based materials (BATT4EU Partnership)</t>
+          <t>Innovative technologies and solutions to improve wind energy systems supporting the Strategic Energy Technology (SET) Plan on wind</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-09-D2-01</t>
+          <t>HORIZON-CL5-2026-09-D3-03</t>
         </is>
       </c>
       <c r="C302" s="3" t="n">
@@ -9268,18 +8413,18 @@
         <v>46280</v>
       </c>
       <c r="E302" s="4" t="n">
-        <v>7100000</v>
+        <v>93000000</v>
       </c>
     </row>
     <row r="303">
       <c r="A303" s="2" t="inlineStr">
         <is>
-          <t>Innovative approaches for the spatial design of neighbourhoods</t>
+          <t>Sustainable, inclusive, affordable and beautiful solutions for thermal comfort in buildings</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-PARTICIPATION-02</t>
+          <t>HORIZON-NEB-2026-01-REGEN-01</t>
         </is>
       </c>
       <c r="C303" s="3" t="n">
@@ -9289,18 +8434,18 @@
         <v>46357</v>
       </c>
       <c r="E303" s="4" t="n">
-        <v>5000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" s="2" t="inlineStr">
         <is>
-          <t>Understanding inhabitant’s experiences of neighbourhoods to support their health and well-being</t>
+          <t>Advancing sustainable maintenance and repair measures for existing buildings</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-PARTICIPATION-03</t>
+          <t>HORIZON-NEB-2026-01-REGEN-02</t>
         </is>
       </c>
       <c r="C304" s="3" t="n">
@@ -9316,12 +8461,12 @@
     <row r="305">
       <c r="A305" s="2" t="inlineStr">
         <is>
-          <t>Understanding capital market dynamics for increased investment in New European Bauhaus projects in neighbourhoods</t>
+          <t>Innovative solutions for the sustainable and beautiful use of vertical space</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-BUSINESS-02</t>
+          <t>HORIZON-NEB-2026-01-REGEN-03</t>
         </is>
       </c>
       <c r="C305" s="3" t="n">
@@ -9331,18 +8476,18 @@
         <v>46357</v>
       </c>
       <c r="E305" s="4" t="n">
-        <v>3500000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" s="2" t="inlineStr">
         <is>
-          <t>Innovative solutions for the sustainable and beautiful use of vertical space</t>
+          <t>Innovative approaches for the spatial design of neighbourhoods</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-REGEN-03</t>
+          <t>HORIZON-NEB-2026-01-PARTICIPATION-02</t>
         </is>
       </c>
       <c r="C306" s="3" t="n">
@@ -9358,12 +8503,12 @@
     <row r="307">
       <c r="A307" s="2" t="inlineStr">
         <is>
-          <t>Approaches to reuse vacant, obsolete or underutilised spaces</t>
+          <t>Understanding inhabitant’s experiences of neighbourhoods to support their health and well-being</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-BUSINESS-03</t>
+          <t>HORIZON-NEB-2026-01-PARTICIPATION-03</t>
         </is>
       </c>
       <c r="C307" s="3" t="n">
@@ -9373,39 +8518,39 @@
         <v>46357</v>
       </c>
       <c r="E307" s="4" t="n">
-        <v>4500000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" s="2" t="inlineStr">
         <is>
-          <t>Sustainable, inclusive, affordable and beautiful solutions for thermal comfort in buildings</t>
+          <t>Advanced data platforms to integrate whole life carbon in building information tools, assessments, and certification (Built4People Partnership)</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-REGEN-01</t>
+          <t>HORIZON-CL5-2026-09-D4-03</t>
         </is>
       </c>
       <c r="C308" s="3" t="n">
         <v>46147</v>
       </c>
       <c r="D308" s="3" t="n">
-        <v>46357</v>
+        <v>46280</v>
       </c>
       <c r="E308" s="4" t="n">
-        <v>4000000</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" s="2" t="inlineStr">
         <is>
-          <t>Advancing sustainable maintenance and repair measures for existing buildings</t>
+          <t>Understanding capital market dynamics for increased investment in New European Bauhaus projects in neighbourhoods</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-REGEN-02</t>
+          <t>HORIZON-NEB-2026-01-BUSINESS-02</t>
         </is>
       </c>
       <c r="C309" s="3" t="n">
@@ -9415,49 +8560,49 @@
         <v>46357</v>
       </c>
       <c r="E309" s="4" t="n">
-        <v>5000000</v>
+        <v>3500000</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="2" t="inlineStr">
         <is>
-          <t>Advanced data platforms to integrate whole life carbon in building information tools, assessments, and certification (Built4People Partnership)</t>
+          <t>Structurally addressing homelessness through coordinated social infrastructure and services in neighbourhoods</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-09-D4-03</t>
+          <t>HORIZON-NEB-2026-01-BUSINESS-01</t>
         </is>
       </c>
       <c r="C310" s="3" t="n">
         <v>46147</v>
       </c>
       <c r="D310" s="3" t="n">
-        <v>46280</v>
+        <v>46357</v>
       </c>
       <c r="E310" s="4" t="n">
-        <v>5250000</v>
+        <v>3500000</v>
       </c>
     </row>
     <row r="311">
       <c r="A311" s="2" t="inlineStr">
         <is>
-          <t>Structurally addressing homelessness through coordinated social infrastructure and services in neighbourhoods</t>
+          <t>Researching the technical, social &amp; economic factors impacting the energy performance of Smart Buildings (Built4People Partnership)</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
         <is>
-          <t>HORIZON-NEB-2026-01-BUSINESS-01</t>
+          <t>HORIZON-CL5-2026-09-D4-01</t>
         </is>
       </c>
       <c r="C311" s="3" t="n">
         <v>46147</v>
       </c>
       <c r="D311" s="3" t="n">
-        <v>46357</v>
+        <v>46280</v>
       </c>
       <c r="E311" s="4" t="n">
-        <v>3500000</v>
+        <v>5250000</v>
       </c>
     </row>
     <row r="312">
@@ -9484,12 +8629,12 @@
     <row r="313">
       <c r="A313" s="2" t="inlineStr">
         <is>
-          <t>Researching the technical, social &amp; economic factors impacting the energy performance of Smart Buildings (Built4People Partnership)</t>
+          <t>Low disturbance prefabrication approaches for deep renovation of multi-storey buildings (Built4People Partnership)</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-09-D4-01</t>
+          <t>HORIZON-CL5-2026-09-D4-02</t>
         </is>
       </c>
       <c r="C313" s="3" t="n">
@@ -9499,18 +8644,18 @@
         <v>46280</v>
       </c>
       <c r="E313" s="4" t="n">
-        <v>5250000</v>
+        <v>7000000</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" s="2" t="inlineStr">
         <is>
-          <t>Low disturbance prefabrication approaches for deep renovation of multi-storey buildings (Built4People Partnership)</t>
+          <t>Full-scale demonstration of heat upgrade solutions in industrial processes</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-09-D4-02</t>
+          <t>HORIZON-CL5-2026-09-D4-08</t>
         </is>
       </c>
       <c r="C314" s="3" t="n">
@@ -9520,18 +8665,18 @@
         <v>46280</v>
       </c>
       <c r="E314" s="4" t="n">
-        <v>7000000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" s="2" t="inlineStr">
         <is>
-          <t>Full-scale demonstration of heat upgrade solutions in industrial processes</t>
+          <t>Coordinated topic with India on recycling of EV batteries</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-09-D4-08</t>
+          <t>HORIZON-CL5-2026-09-D2-04</t>
         </is>
       </c>
       <c r="C315" s="3" t="n">
@@ -9541,18 +8686,18 @@
         <v>46280</v>
       </c>
       <c r="E315" s="4" t="n">
-        <v>9000000</v>
+        <v>9400000</v>
       </c>
     </row>
     <row r="316">
       <c r="A316" s="2" t="inlineStr">
         <is>
-          <t>Innovative technologies and solutions to improve wind energy systems supporting the Strategic Energy Technology (SET) Plan on wind</t>
+          <t>Producing battery-grade materials for electrodes through sustainable processing and refining of raw materials or developing bio-based materials (BATT4EU Partnership)</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
         <is>
-          <t>HORIZON-CL5-2026-09-D3-03</t>
+          <t>HORIZON-CL5-2026-09-D2-01</t>
         </is>
       </c>
       <c r="C316" s="3" t="n">
@@ -9562,7 +8707,7 @@
         <v>46280</v>
       </c>
       <c r="E316" s="4" t="n">
-        <v>93000000</v>
+        <v>7100000</v>
       </c>
     </row>
     <row r="317">
@@ -9589,12 +8734,12 @@
     <row r="318">
       <c r="A318" s="2" t="inlineStr">
         <is>
-          <t>Teaming Synergies</t>
+          <t>Research Management Facility</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
         <is>
-          <t>HORIZON-WIDERA-2026-01-WIDENING-01</t>
+          <t>HORIZON-WIDERA-2026-04-WIDENING-01</t>
         </is>
       </c>
       <c r="C318" s="3" t="n">
@@ -9610,12 +8755,12 @@
     <row r="319">
       <c r="A319" s="2" t="inlineStr">
         <is>
-          <t>Research Management Facility</t>
+          <t>Teaming Synergies</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
         <is>
-          <t>HORIZON-WIDERA-2026-04-WIDENING-01</t>
+          <t>HORIZON-WIDERA-2026-01-WIDENING-01</t>
         </is>
       </c>
       <c r="C319" s="3" t="n">
@@ -9631,12 +8776,12 @@
     <row r="320">
       <c r="A320" s="2" t="inlineStr">
         <is>
-          <t>Advancing the European bio-based innovation enabled by biotechnology and biomanufacturing concepts</t>
+          <t>Pushing the frontier of knowledge and conservation action for deep sea ecosystems</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-07</t>
+          <t>HORIZON-CL6-2026-01-BIODIV-03</t>
         </is>
       </c>
       <c r="C320" s="3" t="n">
@@ -9646,18 +8791,18 @@
         <v>46282</v>
       </c>
       <c r="E320" s="4" t="n">
-        <v>4000000</v>
+        <v>9000000</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" s="2" t="inlineStr">
         <is>
-          <t>Understanding and tackling the decline of insects</t>
+          <t>Advancing integrated scenarios and prediction models for informing transition to a nature positive society</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-BIODIV-01</t>
+          <t>HORIZON-CL6-2026-01-BIODIV-05</t>
         </is>
       </c>
       <c r="C321" s="3" t="n">
@@ -9667,18 +8812,18 @@
         <v>46282</v>
       </c>
       <c r="E321" s="4" t="n">
-        <v>6500000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" s="2" t="inlineStr">
         <is>
-          <t>Supporting pre-normative research for standardization of the bio-based products</t>
+          <t>Ensuring continuous effectiveness of protected areas in conserving habitats and species while facing intensifying drivers of biodiversity loss</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-08</t>
+          <t>HORIZON-CL6-2026-01-BIODIV-04</t>
         </is>
       </c>
       <c r="C322" s="3" t="n">
@@ -9688,7 +8833,7 @@
         <v>46282</v>
       </c>
       <c r="E322" s="4" t="n">
-        <v>4000000</v>
+        <v>6500000</v>
       </c>
     </row>
     <row r="323">
@@ -9715,12 +8860,12 @@
     <row r="324">
       <c r="A324" s="2" t="inlineStr">
         <is>
-          <t>Bio-based innovation in society: supporting the sustainable way of living</t>
+          <t>Improving circularity of multilayer flexible plastic food contact packaging</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-10</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-01</t>
         </is>
       </c>
       <c r="C324" s="3" t="n">
@@ -9730,18 +8875,18 @@
         <v>46282</v>
       </c>
       <c r="E324" s="4" t="n">
-        <v>4000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" s="2" t="inlineStr">
         <is>
-          <t>Ensuring continuous effectiveness of protected areas in conserving habitats and species while facing intensifying drivers of biodiversity loss</t>
+          <t>Understanding biomass flows in Europe</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-BIODIV-04</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-05</t>
         </is>
       </c>
       <c r="C325" s="3" t="n">
@@ -9751,18 +8896,18 @@
         <v>46282</v>
       </c>
       <c r="E325" s="4" t="n">
-        <v>6500000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="326">
       <c r="A326" s="2" t="inlineStr">
         <is>
-          <t>Improving circularity of multilayer flexible plastic food contact packaging</t>
+          <t>Bioeconomy policy support hub for Member States, regions and sectors</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-01</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-06</t>
         </is>
       </c>
       <c r="C326" s="3" t="n">
@@ -9772,18 +8917,18 @@
         <v>46282</v>
       </c>
       <c r="E326" s="4" t="n">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="2" t="inlineStr">
         <is>
-          <t>Developing methods to assess the presence, functions and sensitivity of groundwater ecosystems</t>
+          <t>Advanced recovery of critical raw materials from Waste from Electrical and Electronic Equipment (WEEE)</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-BIODIV-02</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-03</t>
         </is>
       </c>
       <c r="C327" s="3" t="n">
@@ -9799,12 +8944,12 @@
     <row r="328">
       <c r="A328" s="2" t="inlineStr">
         <is>
-          <t>Demonstrating and deploying innovative collection, sorting-for-reuse and repair systems for textiles at city/region level (Circular Cities and Regions Initiative topic)</t>
+          <t>Developing managed aquifer recharge techniques (MAR) in a rural context</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-04</t>
+          <t>HORIZON-CL6-2026-01-ZEROPOLLUTION-03</t>
         </is>
       </c>
       <c r="C328" s="3" t="n">
@@ -9814,18 +8959,18 @@
         <v>46282</v>
       </c>
       <c r="E328" s="4" t="n">
-        <v>5000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="329">
       <c r="A329" s="2" t="inlineStr">
         <is>
-          <t>Pushing the frontier of knowledge and conservation action for deep sea ecosystems</t>
+          <t>Harnessing the unique properties of marine organisms to deliver sustainable blue bio-based products</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-BIODIV-03</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-11</t>
         </is>
       </c>
       <c r="C329" s="3" t="n">
@@ -9835,18 +8980,18 @@
         <v>46282</v>
       </c>
       <c r="E329" s="4" t="n">
-        <v>9000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" s="2" t="inlineStr">
         <is>
-          <t>Boosting agrobiodiversity for food security and sustainable competitiveness</t>
+          <t>Balancing food security, bioeconomy, climate and biodiversity objectives to unlock sustainable value chains</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-BIODIV-06</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-09</t>
         </is>
       </c>
       <c r="C330" s="3" t="n">
@@ -9862,12 +9007,12 @@
     <row r="331">
       <c r="A331" s="2" t="inlineStr">
         <is>
-          <t>Advancing integrated scenarios and prediction models for informing transition to a nature positive society</t>
+          <t>Developing methods to assess the presence, functions and sensitivity of groundwater ecosystems</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-BIODIV-05</t>
+          <t>HORIZON-CL6-2026-01-BIODIV-02</t>
         </is>
       </c>
       <c r="C331" s="3" t="n">
@@ -9883,12 +9028,12 @@
     <row r="332">
       <c r="A332" s="2" t="inlineStr">
         <is>
-          <t>Understanding biomass flows in Europe</t>
+          <t>Demonstrating and deploying innovative collection, sorting-for-reuse and repair systems for textiles at city/region level (Circular Cities and Regions Initiative topic)</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-05</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-04</t>
         </is>
       </c>
       <c r="C332" s="3" t="n">
@@ -9898,18 +9043,18 @@
         <v>46282</v>
       </c>
       <c r="E332" s="4" t="n">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" s="2" t="inlineStr">
         <is>
-          <t>Developing managed aquifer recharge techniques (MAR) in a rural context</t>
+          <t>Bioremediation of Ukraine’s ecosystems contaminated by conflicts</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-ZEROPOLLUTION-03</t>
+          <t>HORIZON-CL6-2026-01-ZEROPOLLUTION-02</t>
         </is>
       </c>
       <c r="C333" s="3" t="n">
@@ -9919,18 +9064,18 @@
         <v>46282</v>
       </c>
       <c r="E333" s="4" t="n">
-        <v>6000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" s="2" t="inlineStr">
         <is>
-          <t>Harnessing the unique properties of marine organisms to deliver sustainable blue bio-based products</t>
+          <t>Advancing the European bio-based innovation enabled by biotechnology and biomanufacturing concepts</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-11</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-07</t>
         </is>
       </c>
       <c r="C334" s="3" t="n">
@@ -9940,18 +9085,18 @@
         <v>46282</v>
       </c>
       <c r="E334" s="4" t="n">
-        <v>5000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" s="2" t="inlineStr">
         <is>
-          <t>Advancing recycling technologies for mixed post-consumer textiles waste from blended products</t>
+          <t>Understanding and tackling the decline of insects</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-02</t>
+          <t>HORIZON-CL6-2026-01-BIODIV-01</t>
         </is>
       </c>
       <c r="C335" s="3" t="n">
@@ -9961,18 +9106,18 @@
         <v>46282</v>
       </c>
       <c r="E335" s="4" t="n">
-        <v>5000000</v>
+        <v>6500000</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" s="2" t="inlineStr">
         <is>
-          <t>Bioeconomy policy support hub for Member States, regions and sectors</t>
+          <t>Bio-based innovation in society: supporting the sustainable way of living</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-06</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-10</t>
         </is>
       </c>
       <c r="C336" s="3" t="n">
@@ -9982,18 +9127,18 @@
         <v>46282</v>
       </c>
       <c r="E336" s="4" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" s="2" t="inlineStr">
         <is>
-          <t>Advanced recovery of critical raw materials from Waste from Electrical and Electronic Equipment (WEEE)</t>
+          <t>Supporting pre-normative research for standardization of the bio-based products</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-03</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-08</t>
         </is>
       </c>
       <c r="C337" s="3" t="n">
@@ -10003,18 +9148,18 @@
         <v>46282</v>
       </c>
       <c r="E337" s="4" t="n">
-        <v>5000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" s="2" t="inlineStr">
         <is>
-          <t>Balancing food security, bioeconomy, climate and biodiversity objectives to unlock sustainable value chains</t>
+          <t>Advancing recycling technologies for mixed post-consumer textiles waste from blended products</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-CIRCBIO-09</t>
+          <t>HORIZON-CL6-2026-01-CIRCBIO-02</t>
         </is>
       </c>
       <c r="C338" s="3" t="n">
@@ -10024,18 +9169,18 @@
         <v>46282</v>
       </c>
       <c r="E338" s="4" t="n">
-        <v>6000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" s="2" t="inlineStr">
         <is>
-          <t>Bioremediation of Ukraine’s ecosystems contaminated by conflicts</t>
+          <t>Boosting agrobiodiversity for food security and sustainable competitiveness</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
         <is>
-          <t>HORIZON-CL6-2026-01-ZEROPOLLUTION-02</t>
+          <t>HORIZON-CL6-2026-01-BIODIV-06</t>
         </is>
       </c>
       <c r="C339" s="3" t="n">
@@ -10045,18 +9190,18 @@
         <v>46282</v>
       </c>
       <c r="E339" s="4" t="n">
-        <v>5000000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" s="2" t="inlineStr">
         <is>
-          <t>MSCA Postdoctoral Fellowships 2026</t>
+          <t>ERA Fellowships</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
         <is>
-          <t>HORIZON-MSCA-2026-PF-01-01</t>
+          <t>HORIZON-WIDERA-2026-05-WIDENING-01</t>
         </is>
       </c>
       <c r="C340" s="3" t="n">
@@ -10065,16 +9210,19 @@
       <c r="D340" s="3" t="n">
         <v>46274</v>
       </c>
+      <c r="E340" s="4" t="n">
+        <v>100000</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" s="2" t="inlineStr">
         <is>
-          <t>ERA Fellowships</t>
+          <t>MSCA Postdoctoral Fellowships 2026</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
         <is>
-          <t>HORIZON-WIDERA-2026-05-WIDENING-01</t>
+          <t>HORIZON-MSCA-2026-PF-01-01</t>
         </is>
       </c>
       <c r="C341" s="3" t="n">
@@ -10083,40 +9231,37 @@
       <c r="D341" s="3" t="n">
         <v>46274</v>
       </c>
-      <c r="E341" s="4" t="n">
-        <v>100000</v>
-      </c>
     </row>
     <row r="342">
       <c r="A342" s="2" t="inlineStr">
         <is>
-          <t>Implementing digital services to empower neuroscience research for health and brain inspired technology via EBRAINS</t>
+          <t>Reinforcing EU autonomous access to space through EU-based spaceports</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
         <is>
-          <t>HORIZON-INFRA-2026-SERV-01-01</t>
+          <t>HORIZON-CL4-2026-SPACE-03-11</t>
         </is>
       </c>
       <c r="C342" s="3" t="n">
         <v>46091</v>
       </c>
       <c r="D342" s="3" t="n">
-        <v>46189</v>
+        <v>46268</v>
       </c>
       <c r="E342" s="4" t="n">
-        <v>32000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="343">
       <c r="A343" s="2" t="inlineStr">
         <is>
-          <t>Strengthening the human capital managing research infrastructures, including in international context</t>
+          <t>Research infrastructure concept development including major upgrades or extensions of existing infrastructures</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
         <is>
-          <t>HORIZON-INFRA-2026-DEV-01-04</t>
+          <t>HORIZON-INFRA-2026-DEV-01-01</t>
         </is>
       </c>
       <c r="C343" s="3" t="n">
@@ -10132,12 +9277,12 @@
     <row r="344">
       <c r="A344" s="2" t="inlineStr">
         <is>
-          <t>Trusted frameworks for secure and efficient data sharing in EOSC (EOSC Partnership)</t>
+          <t>Digital twins and/or their major components for environment, climate and security</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
         <is>
-          <t>HORIZON-INFRA-2026-01-EOSC-02</t>
+          <t>HORIZON-INFRA-2026-TECH-01-02</t>
         </is>
       </c>
       <c r="C344" s="3" t="n">
@@ -10147,18 +9292,18 @@
         <v>46189</v>
       </c>
       <c r="E344" s="4" t="n">
-        <v>3000000</v>
+        <v>5000000</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" s="2" t="inlineStr">
         <is>
-          <t>Consolidation of the research infrastructure landscape – individual support for evolution, long-term sustainability and emerging needs of pan-European research infrastructures</t>
+          <t>Consolidation of the research infrastructure landscape – pilots for strategic coordination, synergies and simplified access pathways, by large thematic clusters of pan-European research infrastructures</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
         <is>
-          <t>HORIZON-INFRA-2026-DEV-01-03</t>
+          <t>HORIZON-INFRA-2026-DEV-01-02</t>
         </is>
       </c>
       <c r="C345" s="3" t="n">
@@ -10168,60 +9313,60 @@
         <v>46189</v>
       </c>
       <c r="E345" s="4" t="n">
-        <v>3000000</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="346">
       <c r="A346" s="2" t="inlineStr">
         <is>
-          <t>Consolidation of the research infrastructure landscape – pilots for strategic coordination, synergies and simplified access pathways, by large thematic clusters of pan-European research infrastructures</t>
+          <t>Scientific analysis and exploitation of space data</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
         <is>
-          <t>HORIZON-INFRA-2026-DEV-01-02</t>
+          <t>HORIZON-CL4-2026-SPACE-03-61</t>
         </is>
       </c>
       <c r="C346" s="3" t="n">
         <v>46091</v>
       </c>
       <c r="D346" s="3" t="n">
-        <v>46189</v>
+        <v>46268</v>
       </c>
       <c r="E346" s="4" t="n">
-        <v>4000000</v>
+        <v>1500000</v>
       </c>
     </row>
     <row r="347">
       <c r="A347" s="2" t="inlineStr">
         <is>
-          <t>Digital twins and/or their major components for environment, climate and security</t>
+          <t>Digital enablers and building-blocks for Earth Observation and Satellite telecommunication for Space solutions (Space Partnership)</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
         <is>
-          <t>HORIZON-INFRA-2026-TECH-01-02</t>
+          <t>HORIZON-CL4-2026-SPACE-03-31</t>
         </is>
       </c>
       <c r="C347" s="3" t="n">
         <v>46091</v>
       </c>
       <c r="D347" s="3" t="n">
-        <v>46189</v>
+        <v>46268</v>
       </c>
       <c r="E347" s="4" t="n">
-        <v>5000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="348">
       <c r="A348" s="2" t="inlineStr">
         <is>
-          <t>Scientific analysis and exploitation of space data</t>
+          <t>Space critical EEE components for EU non-dependence – GaN MMICs mm-Wave Foundations (Phase A): Development and Industrialization of Semi-insulating SiC Substrate Capabilities</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2026-SPACE-03-61</t>
+          <t>HORIZON-CL4-2026-SPACE-03-82</t>
         </is>
       </c>
       <c r="C348" s="3" t="n">
@@ -10231,18 +9376,18 @@
         <v>46268</v>
       </c>
       <c r="E348" s="4" t="n">
-        <v>1500000</v>
+        <v>6000000</v>
       </c>
     </row>
     <row r="349">
       <c r="A349" s="2" t="inlineStr">
         <is>
-          <t>Reinforcing EU autonomous access to space through EU-based spaceports</t>
+          <t>Space critical Equipment for EU non-dependence – Space Refuelling Interface</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2026-SPACE-03-11</t>
+          <t>HORIZON-CL4-2026-SPACE-03-86</t>
         </is>
       </c>
       <c r="C349" s="3" t="n">
@@ -10252,18 +9397,18 @@
         <v>46268</v>
       </c>
       <c r="E349" s="4" t="n">
-        <v>10000000</v>
+        <v>2000000</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" s="2" t="inlineStr">
         <is>
-          <t>Digital enablers and building-blocks for Earth Observation and Satellite telecommunication for Space solutions (Space Partnership)</t>
+          <t>Space critical EEE components for EU non-dependence – Radiation Hard FPGA on 7nm</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2026-SPACE-03-31</t>
+          <t>HORIZON-CL4-2026-SPACE-03-81</t>
         </is>
       </c>
       <c r="C350" s="3" t="n">
@@ -10273,18 +9418,18 @@
         <v>46268</v>
       </c>
       <c r="E350" s="4" t="n">
-        <v>3000000</v>
+        <v>12000000</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" s="2" t="inlineStr">
         <is>
-          <t>Space critical Equipment for EU non-dependence – Space Refuelling Interface</t>
+          <t>Critical Facilities Serving Space EEE components for EU non-dependence – High and Very High Energy Irradiation Test Facility Market Deployment</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
         <is>
-          <t>HORIZON-CL4-2026-SPACE-03-86</t>
+          <t>HORIZON-CL4-2026-SPACE-03-85</t>
         </is>
       </c>
       <c r="C351" s="3" t="n">
@@ -10294,7 +9439,7 @@
         <v>46268</v>
       </c>
       <c r="E351" s="4" t="n">
-        <v>2000000</v>
+        <v>3000000</v>
       </c>
     </row>
     <row r="352">

</xml_diff>